<commit_message>
update data with ground truth mass and plots
</commit_message>
<xml_diff>
--- a/python/output/canon/Results_CCI_2021-11-01_default.xlsx
+++ b/python/output/canon/Results_CCI_2021-11-01_default.xlsx
@@ -5,27 +5,39 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daleblack/Google Drive/dev/MolloiLab/CAC-stanford-data/python/output/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daleblack/Google Drive/dev/MolloiLab/CAC-stanford-data/python/output/canon/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A64D411D-0949-4441-9233-931002A0C7E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF8811DE-8426-AE4C-871C-2F70F302EFF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="500" windowWidth="35560" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Used_data" sheetId="1" r:id="rId1"/>
-    <sheet name="IQ_data" sheetId="2" r:id="rId2"/>
-    <sheet name="NPS" sheetId="3" r:id="rId3"/>
-    <sheet name="MTF" sheetId="4" r:id="rId4"/>
-    <sheet name="ESF" sheetId="5" r:id="rId5"/>
-    <sheet name="Unused_data" sheetId="6" r:id="rId6"/>
+    <sheet name="Ground_truth" sheetId="7" r:id="rId1"/>
+    <sheet name="Used_data" sheetId="1" r:id="rId2"/>
+    <sheet name="IQ_data" sheetId="2" r:id="rId3"/>
+    <sheet name="NPS" sheetId="3" r:id="rId4"/>
+    <sheet name="MTF" sheetId="4" r:id="rId5"/>
+    <sheet name="ESF" sheetId="5" r:id="rId6"/>
+    <sheet name="Unused_data" sheetId="6" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="639" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="657" uniqueCount="73">
   <si>
     <t>Phantom</t>
   </si>
@@ -221,6 +233,30 @@
   <si>
     <t>/Users/daleblack/Google Drive/Datasets/Canon_Aquilion_One_Vision/Small_rep5</t>
   </si>
+  <si>
+    <t>Diameter (mm)</t>
+  </si>
+  <si>
+    <t>Length (mm)</t>
+  </si>
+  <si>
+    <t>Density (mg/mL)</t>
+  </si>
+  <si>
+    <t>Mass (g)</t>
+  </si>
+  <si>
+    <t>gt_diameter (mm)</t>
+  </si>
+  <si>
+    <t>gt_length (mm)</t>
+  </si>
+  <si>
+    <t>gt_density (mg/mL)</t>
+  </si>
+  <si>
+    <t>gt_mass (g)</t>
+  </si>
 </sst>
 </file>
 
@@ -272,6 +308,1577 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>CAC</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Mass vs. Ground Truth Mass (Canon)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Used_data!$R$2:$R$91</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="90"/>
+                <c:pt idx="0">
+                  <c:v>78.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16.956</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.628</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>39.25</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8.4779999999999998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.314</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>19.625</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.2389999999999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.157</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>78.5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>16.956</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.628</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>39.25</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>8.4779999999999998</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.314</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>19.625</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4.2389999999999999</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.157</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>78.5</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>16.956</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.628</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>39.25</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>8.4779999999999998</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.314</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>19.625</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>4.2389999999999999</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.157</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>78.5</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>16.956</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.628</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>39.25</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>8.4779999999999998</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.314</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>19.625</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>4.2389999999999999</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.157</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>78.5</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>16.956</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.628</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>39.25</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>8.4779999999999998</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.314</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>19.625</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>4.2389999999999999</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0.157</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>78.5</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>16.956</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0.628</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>39.25</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>8.4779999999999998</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>0.314</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>19.625</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>4.2389999999999999</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>0.157</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>78.5</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>16.956</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>0.628</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>39.25</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>8.4779999999999998</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>0.314</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>19.625</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>4.2389999999999999</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>0.157</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>78.5</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>16.956</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>0.628</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>39.25</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>8.4779999999999998</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>0.314</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>19.625</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>4.2389999999999999</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>0.157</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>78.5</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>16.956</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>0.628</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>39.25</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>8.4779999999999998</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>0.314</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>19.625</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>4.2389999999999999</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>0.157</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>78.5</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>16.956</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>0.628</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>39.25</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>8.4779999999999998</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>0.314</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>19.625</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>4.2389999999999999</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>0.157</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Used_data!$F$2:$F$91</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="90"/>
+                <c:pt idx="0">
+                  <c:v>94.771150000000006</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20.90344</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.1395200000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>47.790260000000004</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10.88246</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>25.37331</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.7530799999999997</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>87.581609999999998</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>17.548719999999999</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.54747999999999997</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>40.493340000000003</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>8.6439000000000004</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>20.751090000000001</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2.9619499999999999</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>95.991399999999999</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>22.420300000000001</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.89039000000000001</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>52.492280000000001</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>10.29513</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.49265999999999999</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>24.410969999999999</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>6.2665800000000003</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>100.79725999999999</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>24.468810000000001</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.53718999999999995</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>48.345359999999999</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>11.57892</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>25.500170000000001</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>4.6038699999999997</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.30269000000000001</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>95.291749999999993</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>22.792059999999999</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.75600000000000001</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>50.014270000000003</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>11.603579999999999</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.29368</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>26.847580000000001</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>6.6037100000000004</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>99.567989999999995</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>24.67577</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0.66890000000000005</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>49.321469999999998</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>12.762560000000001</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>25.565049999999999</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>5.6934500000000003</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>0.29504000000000002</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>90.848659999999995</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>19.00703</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>0.48315999999999998</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>40.738379999999999</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>8.5130199999999991</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>21.474240000000002</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>2.6876500000000001</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>91.027330000000006</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>19.121729999999999</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>0.30368000000000001</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>40.574240000000003</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>7.6283399999999997</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>20.687169999999998</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>3.9069600000000002</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>85.879859999999994</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>17.681450000000002</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>0.39478999999999997</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>38.607430000000001</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>8.08047</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>20.919350000000001</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>2.9180899999999999</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>88.577690000000004</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>19.290479999999999</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>0.43214000000000002</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>39.428939999999997</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>8.4865100000000009</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>21.60539</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>3.2412899999999998</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-D750-C742-9867-EC9CF8D568F6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="376405264"/>
+        <c:axId val="1238638479"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="376405264"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Ground Truth</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> Mass (g)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1238638479"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1238638479"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Calculated Mass</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> (g)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="376405264"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>501650</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{55E4BDB8-1E86-3342-96BA-FCF40FB5AD28}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -594,11 +2201,210 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F7B8859-2E79-334D-B427-254B762D8618}">
+  <dimension ref="A1:E10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:E10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2">
+        <v>5</v>
+      </c>
+      <c r="C2">
+        <v>5</v>
+      </c>
+      <c r="D2">
+        <v>800</v>
+      </c>
+      <c r="E2">
+        <f>3.14*(B2/2)^2*C2*D2*10^-3</f>
+        <v>78.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3">
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <v>3</v>
+      </c>
+      <c r="D3">
+        <v>800</v>
+      </c>
+      <c r="E3">
+        <f t="shared" ref="E3:E10" si="0">3.14*(B3/2)^2*C3*D3*10^-3</f>
+        <v>16.956</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>800</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="0"/>
+        <v>0.628</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5">
+        <v>5</v>
+      </c>
+      <c r="C5">
+        <v>5</v>
+      </c>
+      <c r="D5">
+        <v>400</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>39.25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6">
+        <v>3</v>
+      </c>
+      <c r="C6">
+        <v>3</v>
+      </c>
+      <c r="D6">
+        <v>400</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>8.4779999999999998</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>400</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>0.314</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8">
+        <v>5</v>
+      </c>
+      <c r="C8">
+        <v>5</v>
+      </c>
+      <c r="D8">
+        <v>200</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>19.625</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9">
+        <v>3</v>
+      </c>
+      <c r="C9">
+        <v>3</v>
+      </c>
+      <c r="D9">
+        <v>200</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>4.2389999999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>200</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>0.157</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N91"/>
+  <dimension ref="A1:R91"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="O1" sqref="O1:R91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -609,9 +2415,13 @@
     <col min="5" max="5" width="12.1640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.1640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="64" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -654,8 +2464,20 @@
       <c r="N1" t="s">
         <v>13</v>
       </c>
+      <c r="O1" t="s">
+        <v>69</v>
+      </c>
+      <c r="P1" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>71</v>
+      </c>
+      <c r="R1" t="s">
+        <v>72</v>
+      </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -698,8 +2520,21 @@
       <c r="N2" t="s">
         <v>15</v>
       </c>
+      <c r="O2">
+        <v>5</v>
+      </c>
+      <c r="P2">
+        <v>5</v>
+      </c>
+      <c r="Q2">
+        <v>800</v>
+      </c>
+      <c r="R2">
+        <f>3.14*(O2/2)^2*P2*Q2*10^-3</f>
+        <v>78.5</v>
+      </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -742,8 +2577,21 @@
       <c r="N3" t="s">
         <v>15</v>
       </c>
+      <c r="O3">
+        <v>3</v>
+      </c>
+      <c r="P3">
+        <v>3</v>
+      </c>
+      <c r="Q3">
+        <v>800</v>
+      </c>
+      <c r="R3">
+        <f t="shared" ref="R3:R19" si="0">3.14*(O3/2)^2*P3*Q3*10^-3</f>
+        <v>16.956</v>
+      </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -786,8 +2634,21 @@
       <c r="N4" t="s">
         <v>15</v>
       </c>
+      <c r="O4">
+        <v>1</v>
+      </c>
+      <c r="P4">
+        <v>1</v>
+      </c>
+      <c r="Q4">
+        <v>800</v>
+      </c>
+      <c r="R4">
+        <f t="shared" si="0"/>
+        <v>0.628</v>
+      </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -830,8 +2691,21 @@
       <c r="N5" t="s">
         <v>15</v>
       </c>
+      <c r="O5">
+        <v>5</v>
+      </c>
+      <c r="P5">
+        <v>5</v>
+      </c>
+      <c r="Q5">
+        <v>400</v>
+      </c>
+      <c r="R5">
+        <f t="shared" si="0"/>
+        <v>39.25</v>
+      </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -874,8 +2748,21 @@
       <c r="N6" t="s">
         <v>15</v>
       </c>
+      <c r="O6">
+        <v>3</v>
+      </c>
+      <c r="P6">
+        <v>3</v>
+      </c>
+      <c r="Q6">
+        <v>400</v>
+      </c>
+      <c r="R6">
+        <f t="shared" si="0"/>
+        <v>8.4779999999999998</v>
+      </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -918,8 +2805,21 @@
       <c r="N7" t="s">
         <v>15</v>
       </c>
+      <c r="O7">
+        <v>1</v>
+      </c>
+      <c r="P7">
+        <v>1</v>
+      </c>
+      <c r="Q7">
+        <v>400</v>
+      </c>
+      <c r="R7">
+        <f t="shared" si="0"/>
+        <v>0.314</v>
+      </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -962,8 +2862,21 @@
       <c r="N8" t="s">
         <v>15</v>
       </c>
+      <c r="O8">
+        <v>5</v>
+      </c>
+      <c r="P8">
+        <v>5</v>
+      </c>
+      <c r="Q8">
+        <v>200</v>
+      </c>
+      <c r="R8">
+        <f t="shared" si="0"/>
+        <v>19.625</v>
+      </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -1006,8 +2919,21 @@
       <c r="N9" t="s">
         <v>15</v>
       </c>
+      <c r="O9">
+        <v>3</v>
+      </c>
+      <c r="P9">
+        <v>3</v>
+      </c>
+      <c r="Q9">
+        <v>200</v>
+      </c>
+      <c r="R9">
+        <f t="shared" si="0"/>
+        <v>4.2389999999999999</v>
+      </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -1050,8 +2976,21 @@
       <c r="N10" t="s">
         <v>15</v>
       </c>
+      <c r="O10">
+        <v>1</v>
+      </c>
+      <c r="P10">
+        <v>1</v>
+      </c>
+      <c r="Q10">
+        <v>200</v>
+      </c>
+      <c r="R10">
+        <f t="shared" si="0"/>
+        <v>0.157</v>
+      </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -1094,8 +3033,21 @@
       <c r="N11" t="s">
         <v>56</v>
       </c>
+      <c r="O11">
+        <v>5</v>
+      </c>
+      <c r="P11">
+        <v>5</v>
+      </c>
+      <c r="Q11">
+        <v>800</v>
+      </c>
+      <c r="R11">
+        <f>3.14*(O11/2)^2*P11*Q11*10^-3</f>
+        <v>78.5</v>
+      </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -1138,8 +3090,21 @@
       <c r="N12" t="s">
         <v>56</v>
       </c>
+      <c r="O12">
+        <v>3</v>
+      </c>
+      <c r="P12">
+        <v>3</v>
+      </c>
+      <c r="Q12">
+        <v>800</v>
+      </c>
+      <c r="R12">
+        <f t="shared" ref="R12:R19" si="1">3.14*(O12/2)^2*P12*Q12*10^-3</f>
+        <v>16.956</v>
+      </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -1182,8 +3147,21 @@
       <c r="N13" t="s">
         <v>56</v>
       </c>
+      <c r="O13">
+        <v>1</v>
+      </c>
+      <c r="P13">
+        <v>1</v>
+      </c>
+      <c r="Q13">
+        <v>800</v>
+      </c>
+      <c r="R13">
+        <f t="shared" si="1"/>
+        <v>0.628</v>
+      </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -1226,8 +3204,21 @@
       <c r="N14" t="s">
         <v>56</v>
       </c>
+      <c r="O14">
+        <v>5</v>
+      </c>
+      <c r="P14">
+        <v>5</v>
+      </c>
+      <c r="Q14">
+        <v>400</v>
+      </c>
+      <c r="R14">
+        <f t="shared" si="1"/>
+        <v>39.25</v>
+      </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -1270,8 +3261,21 @@
       <c r="N15" t="s">
         <v>56</v>
       </c>
+      <c r="O15">
+        <v>3</v>
+      </c>
+      <c r="P15">
+        <v>3</v>
+      </c>
+      <c r="Q15">
+        <v>400</v>
+      </c>
+      <c r="R15">
+        <f t="shared" si="1"/>
+        <v>8.4779999999999998</v>
+      </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -1314,8 +3318,21 @@
       <c r="N16" t="s">
         <v>56</v>
       </c>
+      <c r="O16">
+        <v>1</v>
+      </c>
+      <c r="P16">
+        <v>1</v>
+      </c>
+      <c r="Q16">
+        <v>400</v>
+      </c>
+      <c r="R16">
+        <f t="shared" si="1"/>
+        <v>0.314</v>
+      </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>14</v>
       </c>
@@ -1358,8 +3375,21 @@
       <c r="N17" t="s">
         <v>56</v>
       </c>
+      <c r="O17">
+        <v>5</v>
+      </c>
+      <c r="P17">
+        <v>5</v>
+      </c>
+      <c r="Q17">
+        <v>200</v>
+      </c>
+      <c r="R17">
+        <f t="shared" si="1"/>
+        <v>19.625</v>
+      </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>14</v>
       </c>
@@ -1402,8 +3432,21 @@
       <c r="N18" t="s">
         <v>56</v>
       </c>
+      <c r="O18">
+        <v>3</v>
+      </c>
+      <c r="P18">
+        <v>3</v>
+      </c>
+      <c r="Q18">
+        <v>200</v>
+      </c>
+      <c r="R18">
+        <f t="shared" si="1"/>
+        <v>4.2389999999999999</v>
+      </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>14</v>
       </c>
@@ -1446,8 +3489,21 @@
       <c r="N19" t="s">
         <v>56</v>
       </c>
+      <c r="O19">
+        <v>1</v>
+      </c>
+      <c r="P19">
+        <v>1</v>
+      </c>
+      <c r="Q19">
+        <v>200</v>
+      </c>
+      <c r="R19">
+        <f t="shared" si="1"/>
+        <v>0.157</v>
+      </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>14</v>
       </c>
@@ -1490,8 +3546,21 @@
       <c r="N20" t="s">
         <v>57</v>
       </c>
+      <c r="O20">
+        <v>5</v>
+      </c>
+      <c r="P20">
+        <v>5</v>
+      </c>
+      <c r="Q20">
+        <v>800</v>
+      </c>
+      <c r="R20">
+        <f>3.14*(O20/2)^2*P20*Q20*10^-3</f>
+        <v>78.5</v>
+      </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>14</v>
       </c>
@@ -1534,8 +3603,21 @@
       <c r="N21" t="s">
         <v>57</v>
       </c>
+      <c r="O21">
+        <v>3</v>
+      </c>
+      <c r="P21">
+        <v>3</v>
+      </c>
+      <c r="Q21">
+        <v>800</v>
+      </c>
+      <c r="R21">
+        <f t="shared" ref="R21:R28" si="2">3.14*(O21/2)^2*P21*Q21*10^-3</f>
+        <v>16.956</v>
+      </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>14</v>
       </c>
@@ -1578,8 +3660,21 @@
       <c r="N22" t="s">
         <v>57</v>
       </c>
+      <c r="O22">
+        <v>1</v>
+      </c>
+      <c r="P22">
+        <v>1</v>
+      </c>
+      <c r="Q22">
+        <v>800</v>
+      </c>
+      <c r="R22">
+        <f t="shared" si="2"/>
+        <v>0.628</v>
+      </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>14</v>
       </c>
@@ -1622,8 +3717,21 @@
       <c r="N23" t="s">
         <v>57</v>
       </c>
+      <c r="O23">
+        <v>5</v>
+      </c>
+      <c r="P23">
+        <v>5</v>
+      </c>
+      <c r="Q23">
+        <v>400</v>
+      </c>
+      <c r="R23">
+        <f t="shared" si="2"/>
+        <v>39.25</v>
+      </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>14</v>
       </c>
@@ -1666,8 +3774,21 @@
       <c r="N24" t="s">
         <v>57</v>
       </c>
+      <c r="O24">
+        <v>3</v>
+      </c>
+      <c r="P24">
+        <v>3</v>
+      </c>
+      <c r="Q24">
+        <v>400</v>
+      </c>
+      <c r="R24">
+        <f t="shared" si="2"/>
+        <v>8.4779999999999998</v>
+      </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>14</v>
       </c>
@@ -1710,8 +3831,21 @@
       <c r="N25" t="s">
         <v>57</v>
       </c>
+      <c r="O25">
+        <v>1</v>
+      </c>
+      <c r="P25">
+        <v>1</v>
+      </c>
+      <c r="Q25">
+        <v>400</v>
+      </c>
+      <c r="R25">
+        <f t="shared" si="2"/>
+        <v>0.314</v>
+      </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>14</v>
       </c>
@@ -1754,8 +3888,21 @@
       <c r="N26" t="s">
         <v>57</v>
       </c>
+      <c r="O26">
+        <v>5</v>
+      </c>
+      <c r="P26">
+        <v>5</v>
+      </c>
+      <c r="Q26">
+        <v>200</v>
+      </c>
+      <c r="R26">
+        <f t="shared" si="2"/>
+        <v>19.625</v>
+      </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>14</v>
       </c>
@@ -1798,8 +3945,21 @@
       <c r="N27" t="s">
         <v>57</v>
       </c>
+      <c r="O27">
+        <v>3</v>
+      </c>
+      <c r="P27">
+        <v>3</v>
+      </c>
+      <c r="Q27">
+        <v>200</v>
+      </c>
+      <c r="R27">
+        <f t="shared" si="2"/>
+        <v>4.2389999999999999</v>
+      </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>14</v>
       </c>
@@ -1842,8 +4002,21 @@
       <c r="N28" t="s">
         <v>57</v>
       </c>
+      <c r="O28">
+        <v>1</v>
+      </c>
+      <c r="P28">
+        <v>1</v>
+      </c>
+      <c r="Q28">
+        <v>200</v>
+      </c>
+      <c r="R28">
+        <f t="shared" si="2"/>
+        <v>0.157</v>
+      </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>14</v>
       </c>
@@ -1886,8 +4059,21 @@
       <c r="N29" t="s">
         <v>58</v>
       </c>
+      <c r="O29">
+        <v>5</v>
+      </c>
+      <c r="P29">
+        <v>5</v>
+      </c>
+      <c r="Q29">
+        <v>800</v>
+      </c>
+      <c r="R29">
+        <f>3.14*(O29/2)^2*P29*Q29*10^-3</f>
+        <v>78.5</v>
+      </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>14</v>
       </c>
@@ -1930,8 +4116,21 @@
       <c r="N30" t="s">
         <v>58</v>
       </c>
+      <c r="O30">
+        <v>3</v>
+      </c>
+      <c r="P30">
+        <v>3</v>
+      </c>
+      <c r="Q30">
+        <v>800</v>
+      </c>
+      <c r="R30">
+        <f t="shared" ref="R30:R37" si="3">3.14*(O30/2)^2*P30*Q30*10^-3</f>
+        <v>16.956</v>
+      </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>14</v>
       </c>
@@ -1974,8 +4173,21 @@
       <c r="N31" t="s">
         <v>58</v>
       </c>
+      <c r="O31">
+        <v>1</v>
+      </c>
+      <c r="P31">
+        <v>1</v>
+      </c>
+      <c r="Q31">
+        <v>800</v>
+      </c>
+      <c r="R31">
+        <f t="shared" si="3"/>
+        <v>0.628</v>
+      </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>14</v>
       </c>
@@ -2018,8 +4230,21 @@
       <c r="N32" t="s">
         <v>58</v>
       </c>
+      <c r="O32">
+        <v>5</v>
+      </c>
+      <c r="P32">
+        <v>5</v>
+      </c>
+      <c r="Q32">
+        <v>400</v>
+      </c>
+      <c r="R32">
+        <f t="shared" si="3"/>
+        <v>39.25</v>
+      </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>14</v>
       </c>
@@ -2062,8 +4287,21 @@
       <c r="N33" t="s">
         <v>58</v>
       </c>
+      <c r="O33">
+        <v>3</v>
+      </c>
+      <c r="P33">
+        <v>3</v>
+      </c>
+      <c r="Q33">
+        <v>400</v>
+      </c>
+      <c r="R33">
+        <f t="shared" si="3"/>
+        <v>8.4779999999999998</v>
+      </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>14</v>
       </c>
@@ -2106,8 +4344,21 @@
       <c r="N34" t="s">
         <v>58</v>
       </c>
+      <c r="O34">
+        <v>1</v>
+      </c>
+      <c r="P34">
+        <v>1</v>
+      </c>
+      <c r="Q34">
+        <v>400</v>
+      </c>
+      <c r="R34">
+        <f t="shared" si="3"/>
+        <v>0.314</v>
+      </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>14</v>
       </c>
@@ -2150,8 +4401,21 @@
       <c r="N35" t="s">
         <v>58</v>
       </c>
+      <c r="O35">
+        <v>5</v>
+      </c>
+      <c r="P35">
+        <v>5</v>
+      </c>
+      <c r="Q35">
+        <v>200</v>
+      </c>
+      <c r="R35">
+        <f t="shared" si="3"/>
+        <v>19.625</v>
+      </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>14</v>
       </c>
@@ -2194,8 +4458,21 @@
       <c r="N36" t="s">
         <v>58</v>
       </c>
+      <c r="O36">
+        <v>3</v>
+      </c>
+      <c r="P36">
+        <v>3</v>
+      </c>
+      <c r="Q36">
+        <v>200</v>
+      </c>
+      <c r="R36">
+        <f t="shared" si="3"/>
+        <v>4.2389999999999999</v>
+      </c>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>14</v>
       </c>
@@ -2238,8 +4515,21 @@
       <c r="N37" t="s">
         <v>58</v>
       </c>
+      <c r="O37">
+        <v>1</v>
+      </c>
+      <c r="P37">
+        <v>1</v>
+      </c>
+      <c r="Q37">
+        <v>200</v>
+      </c>
+      <c r="R37">
+        <f t="shared" si="3"/>
+        <v>0.157</v>
+      </c>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>14</v>
       </c>
@@ -2282,8 +4572,21 @@
       <c r="N38" t="s">
         <v>59</v>
       </c>
+      <c r="O38">
+        <v>5</v>
+      </c>
+      <c r="P38">
+        <v>5</v>
+      </c>
+      <c r="Q38">
+        <v>800</v>
+      </c>
+      <c r="R38">
+        <f>3.14*(O38/2)^2*P38*Q38*10^-3</f>
+        <v>78.5</v>
+      </c>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>14</v>
       </c>
@@ -2326,8 +4629,21 @@
       <c r="N39" t="s">
         <v>59</v>
       </c>
+      <c r="O39">
+        <v>3</v>
+      </c>
+      <c r="P39">
+        <v>3</v>
+      </c>
+      <c r="Q39">
+        <v>800</v>
+      </c>
+      <c r="R39">
+        <f t="shared" ref="R39:R46" si="4">3.14*(O39/2)^2*P39*Q39*10^-3</f>
+        <v>16.956</v>
+      </c>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>14</v>
       </c>
@@ -2370,8 +4686,21 @@
       <c r="N40" t="s">
         <v>59</v>
       </c>
+      <c r="O40">
+        <v>1</v>
+      </c>
+      <c r="P40">
+        <v>1</v>
+      </c>
+      <c r="Q40">
+        <v>800</v>
+      </c>
+      <c r="R40">
+        <f t="shared" si="4"/>
+        <v>0.628</v>
+      </c>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>14</v>
       </c>
@@ -2414,8 +4743,21 @@
       <c r="N41" t="s">
         <v>59</v>
       </c>
+      <c r="O41">
+        <v>5</v>
+      </c>
+      <c r="P41">
+        <v>5</v>
+      </c>
+      <c r="Q41">
+        <v>400</v>
+      </c>
+      <c r="R41">
+        <f t="shared" si="4"/>
+        <v>39.25</v>
+      </c>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>14</v>
       </c>
@@ -2458,8 +4800,21 @@
       <c r="N42" t="s">
         <v>59</v>
       </c>
+      <c r="O42">
+        <v>3</v>
+      </c>
+      <c r="P42">
+        <v>3</v>
+      </c>
+      <c r="Q42">
+        <v>400</v>
+      </c>
+      <c r="R42">
+        <f t="shared" si="4"/>
+        <v>8.4779999999999998</v>
+      </c>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>14</v>
       </c>
@@ -2502,8 +4857,21 @@
       <c r="N43" t="s">
         <v>59</v>
       </c>
+      <c r="O43">
+        <v>1</v>
+      </c>
+      <c r="P43">
+        <v>1</v>
+      </c>
+      <c r="Q43">
+        <v>400</v>
+      </c>
+      <c r="R43">
+        <f t="shared" si="4"/>
+        <v>0.314</v>
+      </c>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>14</v>
       </c>
@@ -2546,8 +4914,21 @@
       <c r="N44" t="s">
         <v>59</v>
       </c>
+      <c r="O44">
+        <v>5</v>
+      </c>
+      <c r="P44">
+        <v>5</v>
+      </c>
+      <c r="Q44">
+        <v>200</v>
+      </c>
+      <c r="R44">
+        <f t="shared" si="4"/>
+        <v>19.625</v>
+      </c>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>14</v>
       </c>
@@ -2590,8 +4971,21 @@
       <c r="N45" t="s">
         <v>59</v>
       </c>
+      <c r="O45">
+        <v>3</v>
+      </c>
+      <c r="P45">
+        <v>3</v>
+      </c>
+      <c r="Q45">
+        <v>200</v>
+      </c>
+      <c r="R45">
+        <f t="shared" si="4"/>
+        <v>4.2389999999999999</v>
+      </c>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>14</v>
       </c>
@@ -2634,8 +5028,21 @@
       <c r="N46" t="s">
         <v>59</v>
       </c>
+      <c r="O46">
+        <v>1</v>
+      </c>
+      <c r="P46">
+        <v>1</v>
+      </c>
+      <c r="Q46">
+        <v>200</v>
+      </c>
+      <c r="R46">
+        <f t="shared" si="4"/>
+        <v>0.157</v>
+      </c>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>14</v>
       </c>
@@ -2678,8 +5085,21 @@
       <c r="N47" t="s">
         <v>60</v>
       </c>
+      <c r="O47">
+        <v>5</v>
+      </c>
+      <c r="P47">
+        <v>5</v>
+      </c>
+      <c r="Q47">
+        <v>800</v>
+      </c>
+      <c r="R47">
+        <f>3.14*(O47/2)^2*P47*Q47*10^-3</f>
+        <v>78.5</v>
+      </c>
     </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>14</v>
       </c>
@@ -2722,8 +5142,21 @@
       <c r="N48" t="s">
         <v>60</v>
       </c>
+      <c r="O48">
+        <v>3</v>
+      </c>
+      <c r="P48">
+        <v>3</v>
+      </c>
+      <c r="Q48">
+        <v>800</v>
+      </c>
+      <c r="R48">
+        <f t="shared" ref="R48:R55" si="5">3.14*(O48/2)^2*P48*Q48*10^-3</f>
+        <v>16.956</v>
+      </c>
     </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>14</v>
       </c>
@@ -2766,8 +5199,21 @@
       <c r="N49" t="s">
         <v>60</v>
       </c>
+      <c r="O49">
+        <v>1</v>
+      </c>
+      <c r="P49">
+        <v>1</v>
+      </c>
+      <c r="Q49">
+        <v>800</v>
+      </c>
+      <c r="R49">
+        <f t="shared" si="5"/>
+        <v>0.628</v>
+      </c>
     </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>14</v>
       </c>
@@ -2810,8 +5256,21 @@
       <c r="N50" t="s">
         <v>60</v>
       </c>
+      <c r="O50">
+        <v>5</v>
+      </c>
+      <c r="P50">
+        <v>5</v>
+      </c>
+      <c r="Q50">
+        <v>400</v>
+      </c>
+      <c r="R50">
+        <f t="shared" si="5"/>
+        <v>39.25</v>
+      </c>
     </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>14</v>
       </c>
@@ -2854,8 +5313,21 @@
       <c r="N51" t="s">
         <v>60</v>
       </c>
+      <c r="O51">
+        <v>3</v>
+      </c>
+      <c r="P51">
+        <v>3</v>
+      </c>
+      <c r="Q51">
+        <v>400</v>
+      </c>
+      <c r="R51">
+        <f t="shared" si="5"/>
+        <v>8.4779999999999998</v>
+      </c>
     </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>14</v>
       </c>
@@ -2898,8 +5370,21 @@
       <c r="N52" t="s">
         <v>60</v>
       </c>
+      <c r="O52">
+        <v>1</v>
+      </c>
+      <c r="P52">
+        <v>1</v>
+      </c>
+      <c r="Q52">
+        <v>400</v>
+      </c>
+      <c r="R52">
+        <f t="shared" si="5"/>
+        <v>0.314</v>
+      </c>
     </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>14</v>
       </c>
@@ -2942,8 +5427,21 @@
       <c r="N53" t="s">
         <v>60</v>
       </c>
+      <c r="O53">
+        <v>5</v>
+      </c>
+      <c r="P53">
+        <v>5</v>
+      </c>
+      <c r="Q53">
+        <v>200</v>
+      </c>
+      <c r="R53">
+        <f t="shared" si="5"/>
+        <v>19.625</v>
+      </c>
     </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>14</v>
       </c>
@@ -2986,8 +5484,21 @@
       <c r="N54" t="s">
         <v>60</v>
       </c>
+      <c r="O54">
+        <v>3</v>
+      </c>
+      <c r="P54">
+        <v>3</v>
+      </c>
+      <c r="Q54">
+        <v>200</v>
+      </c>
+      <c r="R54">
+        <f t="shared" si="5"/>
+        <v>4.2389999999999999</v>
+      </c>
     </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>14</v>
       </c>
@@ -3030,8 +5541,21 @@
       <c r="N55" t="s">
         <v>60</v>
       </c>
+      <c r="O55">
+        <v>1</v>
+      </c>
+      <c r="P55">
+        <v>1</v>
+      </c>
+      <c r="Q55">
+        <v>200</v>
+      </c>
+      <c r="R55">
+        <f t="shared" si="5"/>
+        <v>0.157</v>
+      </c>
     </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>14</v>
       </c>
@@ -3074,8 +5598,21 @@
       <c r="N56" t="s">
         <v>61</v>
       </c>
+      <c r="O56">
+        <v>5</v>
+      </c>
+      <c r="P56">
+        <v>5</v>
+      </c>
+      <c r="Q56">
+        <v>800</v>
+      </c>
+      <c r="R56">
+        <f>3.14*(O56/2)^2*P56*Q56*10^-3</f>
+        <v>78.5</v>
+      </c>
     </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>14</v>
       </c>
@@ -3118,8 +5655,21 @@
       <c r="N57" t="s">
         <v>61</v>
       </c>
+      <c r="O57">
+        <v>3</v>
+      </c>
+      <c r="P57">
+        <v>3</v>
+      </c>
+      <c r="Q57">
+        <v>800</v>
+      </c>
+      <c r="R57">
+        <f t="shared" ref="R57:R64" si="6">3.14*(O57/2)^2*P57*Q57*10^-3</f>
+        <v>16.956</v>
+      </c>
     </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>14</v>
       </c>
@@ -3162,8 +5712,21 @@
       <c r="N58" t="s">
         <v>61</v>
       </c>
+      <c r="O58">
+        <v>1</v>
+      </c>
+      <c r="P58">
+        <v>1</v>
+      </c>
+      <c r="Q58">
+        <v>800</v>
+      </c>
+      <c r="R58">
+        <f t="shared" si="6"/>
+        <v>0.628</v>
+      </c>
     </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>14</v>
       </c>
@@ -3206,8 +5769,21 @@
       <c r="N59" t="s">
         <v>61</v>
       </c>
+      <c r="O59">
+        <v>5</v>
+      </c>
+      <c r="P59">
+        <v>5</v>
+      </c>
+      <c r="Q59">
+        <v>400</v>
+      </c>
+      <c r="R59">
+        <f t="shared" si="6"/>
+        <v>39.25</v>
+      </c>
     </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>14</v>
       </c>
@@ -3250,8 +5826,21 @@
       <c r="N60" t="s">
         <v>61</v>
       </c>
+      <c r="O60">
+        <v>3</v>
+      </c>
+      <c r="P60">
+        <v>3</v>
+      </c>
+      <c r="Q60">
+        <v>400</v>
+      </c>
+      <c r="R60">
+        <f t="shared" si="6"/>
+        <v>8.4779999999999998</v>
+      </c>
     </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>14</v>
       </c>
@@ -3294,8 +5883,21 @@
       <c r="N61" t="s">
         <v>61</v>
       </c>
+      <c r="O61">
+        <v>1</v>
+      </c>
+      <c r="P61">
+        <v>1</v>
+      </c>
+      <c r="Q61">
+        <v>400</v>
+      </c>
+      <c r="R61">
+        <f t="shared" si="6"/>
+        <v>0.314</v>
+      </c>
     </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>14</v>
       </c>
@@ -3338,8 +5940,21 @@
       <c r="N62" t="s">
         <v>61</v>
       </c>
+      <c r="O62">
+        <v>5</v>
+      </c>
+      <c r="P62">
+        <v>5</v>
+      </c>
+      <c r="Q62">
+        <v>200</v>
+      </c>
+      <c r="R62">
+        <f t="shared" si="6"/>
+        <v>19.625</v>
+      </c>
     </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>14</v>
       </c>
@@ -3382,8 +5997,21 @@
       <c r="N63" t="s">
         <v>61</v>
       </c>
+      <c r="O63">
+        <v>3</v>
+      </c>
+      <c r="P63">
+        <v>3</v>
+      </c>
+      <c r="Q63">
+        <v>200</v>
+      </c>
+      <c r="R63">
+        <f t="shared" si="6"/>
+        <v>4.2389999999999999</v>
+      </c>
     </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>14</v>
       </c>
@@ -3426,8 +6054,21 @@
       <c r="N64" t="s">
         <v>61</v>
       </c>
+      <c r="O64">
+        <v>1</v>
+      </c>
+      <c r="P64">
+        <v>1</v>
+      </c>
+      <c r="Q64">
+        <v>200</v>
+      </c>
+      <c r="R64">
+        <f t="shared" si="6"/>
+        <v>0.157</v>
+      </c>
     </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>14</v>
       </c>
@@ -3470,8 +6111,21 @@
       <c r="N65" t="s">
         <v>62</v>
       </c>
+      <c r="O65">
+        <v>5</v>
+      </c>
+      <c r="P65">
+        <v>5</v>
+      </c>
+      <c r="Q65">
+        <v>800</v>
+      </c>
+      <c r="R65">
+        <f>3.14*(O65/2)^2*P65*Q65*10^-3</f>
+        <v>78.5</v>
+      </c>
     </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>14</v>
       </c>
@@ -3514,8 +6168,21 @@
       <c r="N66" t="s">
         <v>62</v>
       </c>
+      <c r="O66">
+        <v>3</v>
+      </c>
+      <c r="P66">
+        <v>3</v>
+      </c>
+      <c r="Q66">
+        <v>800</v>
+      </c>
+      <c r="R66">
+        <f t="shared" ref="R66:R73" si="7">3.14*(O66/2)^2*P66*Q66*10^-3</f>
+        <v>16.956</v>
+      </c>
     </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>14</v>
       </c>
@@ -3558,8 +6225,21 @@
       <c r="N67" t="s">
         <v>62</v>
       </c>
+      <c r="O67">
+        <v>1</v>
+      </c>
+      <c r="P67">
+        <v>1</v>
+      </c>
+      <c r="Q67">
+        <v>800</v>
+      </c>
+      <c r="R67">
+        <f t="shared" si="7"/>
+        <v>0.628</v>
+      </c>
     </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>14</v>
       </c>
@@ -3602,8 +6282,21 @@
       <c r="N68" t="s">
         <v>62</v>
       </c>
+      <c r="O68">
+        <v>5</v>
+      </c>
+      <c r="P68">
+        <v>5</v>
+      </c>
+      <c r="Q68">
+        <v>400</v>
+      </c>
+      <c r="R68">
+        <f t="shared" si="7"/>
+        <v>39.25</v>
+      </c>
     </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>14</v>
       </c>
@@ -3646,8 +6339,21 @@
       <c r="N69" t="s">
         <v>62</v>
       </c>
+      <c r="O69">
+        <v>3</v>
+      </c>
+      <c r="P69">
+        <v>3</v>
+      </c>
+      <c r="Q69">
+        <v>400</v>
+      </c>
+      <c r="R69">
+        <f t="shared" si="7"/>
+        <v>8.4779999999999998</v>
+      </c>
     </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>14</v>
       </c>
@@ -3690,8 +6396,21 @@
       <c r="N70" t="s">
         <v>62</v>
       </c>
+      <c r="O70">
+        <v>1</v>
+      </c>
+      <c r="P70">
+        <v>1</v>
+      </c>
+      <c r="Q70">
+        <v>400</v>
+      </c>
+      <c r="R70">
+        <f t="shared" si="7"/>
+        <v>0.314</v>
+      </c>
     </row>
-    <row r="71" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>14</v>
       </c>
@@ -3734,8 +6453,21 @@
       <c r="N71" t="s">
         <v>62</v>
       </c>
+      <c r="O71">
+        <v>5</v>
+      </c>
+      <c r="P71">
+        <v>5</v>
+      </c>
+      <c r="Q71">
+        <v>200</v>
+      </c>
+      <c r="R71">
+        <f t="shared" si="7"/>
+        <v>19.625</v>
+      </c>
     </row>
-    <row r="72" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>14</v>
       </c>
@@ -3778,8 +6510,21 @@
       <c r="N72" t="s">
         <v>62</v>
       </c>
+      <c r="O72">
+        <v>3</v>
+      </c>
+      <c r="P72">
+        <v>3</v>
+      </c>
+      <c r="Q72">
+        <v>200</v>
+      </c>
+      <c r="R72">
+        <f t="shared" si="7"/>
+        <v>4.2389999999999999</v>
+      </c>
     </row>
-    <row r="73" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>14</v>
       </c>
@@ -3822,8 +6567,21 @@
       <c r="N73" t="s">
         <v>62</v>
       </c>
+      <c r="O73">
+        <v>1</v>
+      </c>
+      <c r="P73">
+        <v>1</v>
+      </c>
+      <c r="Q73">
+        <v>200</v>
+      </c>
+      <c r="R73">
+        <f t="shared" si="7"/>
+        <v>0.157</v>
+      </c>
     </row>
-    <row r="74" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>14</v>
       </c>
@@ -3866,8 +6624,21 @@
       <c r="N74" t="s">
         <v>63</v>
       </c>
+      <c r="O74">
+        <v>5</v>
+      </c>
+      <c r="P74">
+        <v>5</v>
+      </c>
+      <c r="Q74">
+        <v>800</v>
+      </c>
+      <c r="R74">
+        <f>3.14*(O74/2)^2*P74*Q74*10^-3</f>
+        <v>78.5</v>
+      </c>
     </row>
-    <row r="75" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>14</v>
       </c>
@@ -3910,8 +6681,21 @@
       <c r="N75" t="s">
         <v>63</v>
       </c>
+      <c r="O75">
+        <v>3</v>
+      </c>
+      <c r="P75">
+        <v>3</v>
+      </c>
+      <c r="Q75">
+        <v>800</v>
+      </c>
+      <c r="R75">
+        <f t="shared" ref="R75:R82" si="8">3.14*(O75/2)^2*P75*Q75*10^-3</f>
+        <v>16.956</v>
+      </c>
     </row>
-    <row r="76" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>14</v>
       </c>
@@ -3954,8 +6738,21 @@
       <c r="N76" t="s">
         <v>63</v>
       </c>
+      <c r="O76">
+        <v>1</v>
+      </c>
+      <c r="P76">
+        <v>1</v>
+      </c>
+      <c r="Q76">
+        <v>800</v>
+      </c>
+      <c r="R76">
+        <f t="shared" si="8"/>
+        <v>0.628</v>
+      </c>
     </row>
-    <row r="77" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>14</v>
       </c>
@@ -3998,8 +6795,21 @@
       <c r="N77" t="s">
         <v>63</v>
       </c>
+      <c r="O77">
+        <v>5</v>
+      </c>
+      <c r="P77">
+        <v>5</v>
+      </c>
+      <c r="Q77">
+        <v>400</v>
+      </c>
+      <c r="R77">
+        <f t="shared" si="8"/>
+        <v>39.25</v>
+      </c>
     </row>
-    <row r="78" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>14</v>
       </c>
@@ -4042,8 +6852,21 @@
       <c r="N78" t="s">
         <v>63</v>
       </c>
+      <c r="O78">
+        <v>3</v>
+      </c>
+      <c r="P78">
+        <v>3</v>
+      </c>
+      <c r="Q78">
+        <v>400</v>
+      </c>
+      <c r="R78">
+        <f t="shared" si="8"/>
+        <v>8.4779999999999998</v>
+      </c>
     </row>
-    <row r="79" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>14</v>
       </c>
@@ -4086,8 +6909,21 @@
       <c r="N79" t="s">
         <v>63</v>
       </c>
+      <c r="O79">
+        <v>1</v>
+      </c>
+      <c r="P79">
+        <v>1</v>
+      </c>
+      <c r="Q79">
+        <v>400</v>
+      </c>
+      <c r="R79">
+        <f t="shared" si="8"/>
+        <v>0.314</v>
+      </c>
     </row>
-    <row r="80" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>14</v>
       </c>
@@ -4130,8 +6966,21 @@
       <c r="N80" t="s">
         <v>63</v>
       </c>
+      <c r="O80">
+        <v>5</v>
+      </c>
+      <c r="P80">
+        <v>5</v>
+      </c>
+      <c r="Q80">
+        <v>200</v>
+      </c>
+      <c r="R80">
+        <f t="shared" si="8"/>
+        <v>19.625</v>
+      </c>
     </row>
-    <row r="81" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>14</v>
       </c>
@@ -4174,8 +7023,21 @@
       <c r="N81" t="s">
         <v>63</v>
       </c>
+      <c r="O81">
+        <v>3</v>
+      </c>
+      <c r="P81">
+        <v>3</v>
+      </c>
+      <c r="Q81">
+        <v>200</v>
+      </c>
+      <c r="R81">
+        <f t="shared" si="8"/>
+        <v>4.2389999999999999</v>
+      </c>
     </row>
-    <row r="82" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>14</v>
       </c>
@@ -4218,8 +7080,21 @@
       <c r="N82" t="s">
         <v>63</v>
       </c>
+      <c r="O82">
+        <v>1</v>
+      </c>
+      <c r="P82">
+        <v>1</v>
+      </c>
+      <c r="Q82">
+        <v>200</v>
+      </c>
+      <c r="R82">
+        <f t="shared" si="8"/>
+        <v>0.157</v>
+      </c>
     </row>
-    <row r="83" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>14</v>
       </c>
@@ -4262,8 +7137,21 @@
       <c r="N83" t="s">
         <v>64</v>
       </c>
+      <c r="O83">
+        <v>5</v>
+      </c>
+      <c r="P83">
+        <v>5</v>
+      </c>
+      <c r="Q83">
+        <v>800</v>
+      </c>
+      <c r="R83">
+        <f>3.14*(O83/2)^2*P83*Q83*10^-3</f>
+        <v>78.5</v>
+      </c>
     </row>
-    <row r="84" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>14</v>
       </c>
@@ -4306,8 +7194,21 @@
       <c r="N84" t="s">
         <v>64</v>
       </c>
+      <c r="O84">
+        <v>3</v>
+      </c>
+      <c r="P84">
+        <v>3</v>
+      </c>
+      <c r="Q84">
+        <v>800</v>
+      </c>
+      <c r="R84">
+        <f t="shared" ref="R84:R91" si="9">3.14*(O84/2)^2*P84*Q84*10^-3</f>
+        <v>16.956</v>
+      </c>
     </row>
-    <row r="85" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>14</v>
       </c>
@@ -4350,8 +7251,21 @@
       <c r="N85" t="s">
         <v>64</v>
       </c>
+      <c r="O85">
+        <v>1</v>
+      </c>
+      <c r="P85">
+        <v>1</v>
+      </c>
+      <c r="Q85">
+        <v>800</v>
+      </c>
+      <c r="R85">
+        <f t="shared" si="9"/>
+        <v>0.628</v>
+      </c>
     </row>
-    <row r="86" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>14</v>
       </c>
@@ -4394,8 +7308,21 @@
       <c r="N86" t="s">
         <v>64</v>
       </c>
+      <c r="O86">
+        <v>5</v>
+      </c>
+      <c r="P86">
+        <v>5</v>
+      </c>
+      <c r="Q86">
+        <v>400</v>
+      </c>
+      <c r="R86">
+        <f t="shared" si="9"/>
+        <v>39.25</v>
+      </c>
     </row>
-    <row r="87" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>14</v>
       </c>
@@ -4438,8 +7365,21 @@
       <c r="N87" t="s">
         <v>64</v>
       </c>
+      <c r="O87">
+        <v>3</v>
+      </c>
+      <c r="P87">
+        <v>3</v>
+      </c>
+      <c r="Q87">
+        <v>400</v>
+      </c>
+      <c r="R87">
+        <f t="shared" si="9"/>
+        <v>8.4779999999999998</v>
+      </c>
     </row>
-    <row r="88" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>14</v>
       </c>
@@ -4482,8 +7422,21 @@
       <c r="N88" t="s">
         <v>64</v>
       </c>
+      <c r="O88">
+        <v>1</v>
+      </c>
+      <c r="P88">
+        <v>1</v>
+      </c>
+      <c r="Q88">
+        <v>400</v>
+      </c>
+      <c r="R88">
+        <f t="shared" si="9"/>
+        <v>0.314</v>
+      </c>
     </row>
-    <row r="89" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>14</v>
       </c>
@@ -4526,8 +7479,21 @@
       <c r="N89" t="s">
         <v>64</v>
       </c>
+      <c r="O89">
+        <v>5</v>
+      </c>
+      <c r="P89">
+        <v>5</v>
+      </c>
+      <c r="Q89">
+        <v>200</v>
+      </c>
+      <c r="R89">
+        <f t="shared" si="9"/>
+        <v>19.625</v>
+      </c>
     </row>
-    <row r="90" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>14</v>
       </c>
@@ -4570,8 +7536,21 @@
       <c r="N90" t="s">
         <v>64</v>
       </c>
+      <c r="O90">
+        <v>3</v>
+      </c>
+      <c r="P90">
+        <v>3</v>
+      </c>
+      <c r="Q90">
+        <v>200</v>
+      </c>
+      <c r="R90">
+        <f t="shared" si="9"/>
+        <v>4.2389999999999999</v>
+      </c>
     </row>
-    <row r="91" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>14</v>
       </c>
@@ -4613,14 +7592,28 @@
       </c>
       <c r="N91" t="s">
         <v>64</v>
+      </c>
+      <c r="O91">
+        <v>1</v>
+      </c>
+      <c r="P91">
+        <v>1</v>
+      </c>
+      <c r="Q91">
+        <v>200</v>
+      </c>
+      <c r="R91">
+        <f t="shared" si="9"/>
+        <v>0.157</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z11"/>
   <sheetViews>
@@ -5429,7 +8422,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AW21"/>
   <sheetViews>
@@ -8433,7 +11426,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:EA21"/>
   <sheetViews>
@@ -16357,7 +19350,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:JB21"/>
   <sheetViews>
@@ -32141,7 +35134,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>

<commit_message>
Deploying to gh-pages from  @ 28a2d09ecce5d18dc37a9decad6b36fcafac56d3 🚀
</commit_message>
<xml_diff>
--- a/python/output/canon/Results_CCI_2021-11-01_default.xlsx
+++ b/python/output/canon/Results_CCI_2021-11-01_default.xlsx
@@ -1,25 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daleblack/Google Drive/dev/MolloiLab/CAC-stanford-data/python/output/canon/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF8811DE-8426-AE4C-871C-2F70F302EFF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35686322-4E30-4242-A341-9DECF6F8A19B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ground_truth" sheetId="7" r:id="rId1"/>
     <sheet name="Used_data" sheetId="1" r:id="rId2"/>
-    <sheet name="IQ_data" sheetId="2" r:id="rId3"/>
-    <sheet name="NPS" sheetId="3" r:id="rId4"/>
-    <sheet name="MTF" sheetId="4" r:id="rId5"/>
-    <sheet name="ESF" sheetId="5" r:id="rId6"/>
-    <sheet name="Unused_data" sheetId="6" r:id="rId7"/>
+    <sheet name="Sheet1" sheetId="8" r:id="rId3"/>
+    <sheet name="IQ_data" sheetId="2" r:id="rId4"/>
+    <sheet name="NPS" sheetId="3" r:id="rId5"/>
+    <sheet name="MTF" sheetId="4" r:id="rId6"/>
+    <sheet name="ESF" sheetId="5" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="657" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="661" uniqueCount="77">
   <si>
     <t>Phantom</t>
   </si>
@@ -257,18 +257,36 @@
   <si>
     <t>gt_mass (g)</t>
   </si>
+  <si>
+    <t>integrated_mass (mg)</t>
+  </si>
+  <si>
+    <t>Small</t>
+  </si>
+  <si>
+    <t>Medium</t>
+  </si>
+  <si>
+    <t>Large</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -291,8 +309,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1284,7 +1303,463 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>High Density (800 mg/cc)</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:strRef>
+              <c:f>Used_data!$T$74:$T$76</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Small</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Medium</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Large</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Used_data!$S$74:$S$76</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>80.053949090000003</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16.68630581</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.65887652529999996</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-4B73-F341-B27D-1893DCF49ECD}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Medium Density (400 mg/cc)</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:strRef>
+              <c:f>Used_data!$T$74:$T$76</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Small</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Medium</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Large</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Used_data!$S$77:$S$79</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>39.46611635</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.7136667069999998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.33023365970000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-4B73-F341-B27D-1893DCF49ECD}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Low Density (200 mg/cc)</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:strRef>
+              <c:f>Used_data!$T$74:$T$76</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Small</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Medium</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Large</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Used_data!$S$80:$S$82</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>20.78860989</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.4722045699999997</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.0228253980000003E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-4B73-F341-B27D-1893DCF49ECD}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="510069472"/>
+        <c:axId val="510020208"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="510069472"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="510020208"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="510020208"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="510069472"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1840,20 +2315,536 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>501650</xdr:colOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>603250</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>29</xdr:col>
-      <xdr:colOff>419100</xdr:colOff>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>520700</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:rowOff>158750</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1873,6 +2864,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>514350</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>374650</xdr:colOff>
+      <xdr:row>84</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E1AEF69E-7488-0946-BB8E-98E5A6820AFE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2401,10 +3428,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R91"/>
+  <dimension ref="A1:U91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="O1" sqref="O1:R91"/>
+    <sheetView tabSelected="1" topLeftCell="B58" workbookViewId="0">
+      <selection activeCell="F74" sqref="F74:F82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2419,9 +3446,10 @@
     <col min="15" max="15" width="12.5" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="17.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2476,8 +3504,11 @@
       <c r="R1" t="s">
         <v>72</v>
       </c>
+      <c r="S1" t="s">
+        <v>73</v>
+      </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -2534,7 +3565,7 @@
         <v>78.5</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -2587,11 +3618,11 @@
         <v>800</v>
       </c>
       <c r="R3">
-        <f t="shared" ref="R3:R19" si="0">3.14*(O3/2)^2*P3*Q3*10^-3</f>
+        <f t="shared" ref="R3:R10" si="0">3.14*(O3/2)^2*P3*Q3*10^-3</f>
         <v>16.956</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -2648,7 +3679,7 @@
         <v>0.628</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -2705,7 +3736,7 @@
         <v>39.25</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -2762,7 +3793,7 @@
         <v>8.4779999999999998</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -2819,7 +3850,7 @@
         <v>0.314</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -2876,7 +3907,7 @@
         <v>19.625</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -2933,7 +3964,7 @@
         <v>4.2389999999999999</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -2990,7 +4021,7 @@
         <v>0.157</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -3047,7 +4078,7 @@
         <v>78.5</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -3104,7 +4135,7 @@
         <v>16.956</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -3161,7 +4192,7 @@
         <v>0.628</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -3218,7 +4249,7 @@
         <v>39.25</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -3275,7 +4306,7 @@
         <v>8.4779999999999998</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -6068,7 +7099,7 @@
         <v>0.157</v>
       </c>
     </row>
-    <row r="65" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>14</v>
       </c>
@@ -6125,7 +7156,7 @@
         <v>78.5</v>
       </c>
     </row>
-    <row r="66" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>14</v>
       </c>
@@ -6182,7 +7213,7 @@
         <v>16.956</v>
       </c>
     </row>
-    <row r="67" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>14</v>
       </c>
@@ -6239,7 +7270,7 @@
         <v>0.628</v>
       </c>
     </row>
-    <row r="68" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>14</v>
       </c>
@@ -6296,7 +7327,7 @@
         <v>39.25</v>
       </c>
     </row>
-    <row r="69" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>14</v>
       </c>
@@ -6353,7 +7384,7 @@
         <v>8.4779999999999998</v>
       </c>
     </row>
-    <row r="70" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>14</v>
       </c>
@@ -6410,7 +7441,7 @@
         <v>0.314</v>
       </c>
     </row>
-    <row r="71" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>14</v>
       </c>
@@ -6467,7 +7498,7 @@
         <v>19.625</v>
       </c>
     </row>
-    <row r="72" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>14</v>
       </c>
@@ -6524,7 +7555,7 @@
         <v>4.2389999999999999</v>
       </c>
     </row>
-    <row r="73" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>14</v>
       </c>
@@ -6581,7 +7612,7 @@
         <v>0.157</v>
       </c>
     </row>
-    <row r="74" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>14</v>
       </c>
@@ -6637,8 +7668,14 @@
         <f>3.14*(O74/2)^2*P74*Q74*10^-3</f>
         <v>78.5</v>
       </c>
+      <c r="S74" s="1">
+        <v>80.053949090000003</v>
+      </c>
+      <c r="T74" t="s">
+        <v>74</v>
+      </c>
     </row>
-    <row r="75" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>14</v>
       </c>
@@ -6694,8 +7731,15 @@
         <f t="shared" ref="R75:R82" si="8">3.14*(O75/2)^2*P75*Q75*10^-3</f>
         <v>16.956</v>
       </c>
+      <c r="S75" s="1">
+        <v>16.68630581</v>
+      </c>
+      <c r="T75" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="U75" s="1"/>
     </row>
-    <row r="76" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>14</v>
       </c>
@@ -6751,8 +7795,15 @@
         <f t="shared" si="8"/>
         <v>0.628</v>
       </c>
+      <c r="S76" s="1">
+        <v>0.65887652529999996</v>
+      </c>
+      <c r="T76" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="U76" s="1"/>
     </row>
-    <row r="77" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>14</v>
       </c>
@@ -6808,8 +7859,11 @@
         <f t="shared" si="8"/>
         <v>39.25</v>
       </c>
+      <c r="S77" s="1">
+        <v>39.46611635</v>
+      </c>
     </row>
-    <row r="78" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>14</v>
       </c>
@@ -6865,8 +7919,11 @@
         <f t="shared" si="8"/>
         <v>8.4779999999999998</v>
       </c>
+      <c r="S78" s="1">
+        <v>7.7136667069999998</v>
+      </c>
     </row>
-    <row r="79" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>14</v>
       </c>
@@ -6922,8 +7979,11 @@
         <f t="shared" si="8"/>
         <v>0.314</v>
       </c>
+      <c r="S79" s="1">
+        <v>0.33023365970000002</v>
+      </c>
     </row>
-    <row r="80" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>14</v>
       </c>
@@ -6979,8 +8039,11 @@
         <f t="shared" si="8"/>
         <v>19.625</v>
       </c>
+      <c r="S80" s="1">
+        <v>20.78860989</v>
+      </c>
     </row>
-    <row r="81" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>14</v>
       </c>
@@ -7036,8 +8099,11 @@
         <f t="shared" si="8"/>
         <v>4.2389999999999999</v>
       </c>
+      <c r="S81" s="1">
+        <v>4.4722045699999997</v>
+      </c>
     </row>
-    <row r="82" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>14</v>
       </c>
@@ -7093,8 +8159,11 @@
         <f t="shared" si="8"/>
         <v>0.157</v>
       </c>
+      <c r="S82" s="1">
+        <v>4.0228253980000003E-2</v>
+      </c>
     </row>
-    <row r="83" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>14</v>
       </c>
@@ -7151,7 +8220,7 @@
         <v>78.5</v>
       </c>
     </row>
-    <row r="84" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>14</v>
       </c>
@@ -7208,7 +8277,7 @@
         <v>16.956</v>
       </c>
     </row>
-    <row r="85" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>14</v>
       </c>
@@ -7265,7 +8334,7 @@
         <v>0.628</v>
       </c>
     </row>
-    <row r="86" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>14</v>
       </c>
@@ -7322,7 +8391,7 @@
         <v>39.25</v>
       </c>
     </row>
-    <row r="87" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>14</v>
       </c>
@@ -7379,7 +8448,7 @@
         <v>8.4779999999999998</v>
       </c>
     </row>
-    <row r="88" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>14</v>
       </c>
@@ -7436,7 +8505,7 @@
         <v>0.314</v>
       </c>
     </row>
-    <row r="89" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>14</v>
       </c>
@@ -7493,7 +8562,7 @@
         <v>19.625</v>
       </c>
     </row>
-    <row r="90" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>14</v>
       </c>
@@ -7550,7 +8619,7 @@
         <v>4.2389999999999999</v>
       </c>
     </row>
-    <row r="91" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>14</v>
       </c>
@@ -7609,11 +8678,24 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5B33EAC-FF24-5D4F-A92B-EE1059DD1E56}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z11"/>
   <sheetViews>
@@ -8422,7 +9504,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AW21"/>
   <sheetViews>
@@ -11426,7 +12508,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:EA21"/>
   <sheetViews>
@@ -19350,11 +20432,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:JB21"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="AG2" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -35132,16 +36214,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>